<commit_message>
BalayPasilungan 9-28-17 *expense.cs - Partial working donation report (no total
</commit_message>
<xml_diff>
--- a/PDF sample & excel/test.xlsx
+++ b/PDF sample & excel/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>DONATIONS SUMMARY REPORT</t>
   </si>
@@ -41,10 +41,13 @@
     <t>IN-KIND</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>test2</t>
   </si>
   <si>
-    <t>-</t>
+    <t>test3</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -123,7 +127,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -424,86 +434,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="7">
+        <v>43002</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="9">
+        <v>150</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>43004</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="12">
         <v>5000</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="12">
+        <v>500000</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>43004</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="9">
-        <v>500000</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="8"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>43005</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="17">
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:I8"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A4:D4"/>
@@ -511,7 +564,7 @@
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>